<commit_message>
finished confusion matrix stuff
</commit_message>
<xml_diff>
--- a/FSCVA/testing.xlsx
+++ b/FSCVA/testing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicklausauen/Desktop/School - 16th/Senior Project/virtual_assistant/Best_Senior_Project/FSCVA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B643CB91-90E1-B747-A880-DEA3E3284A76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBEC3E1C-201E-9A4E-8898-2F63AE8841B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{873E931C-B0B5-5545-B3A4-79196CD8E536}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="179">
   <si>
     <t>get_weather</t>
   </si>
@@ -546,6 +546,33 @@
   </si>
   <si>
     <t>google the scp foundation</t>
+  </si>
+  <si>
+    <t>unknown</t>
+  </si>
+  <si>
+    <t>Nitwit! Blubber! Oddment! Tweak</t>
+  </si>
+  <si>
+    <t>osteoporosis</t>
+  </si>
+  <si>
+    <t>the cake is a lie</t>
+  </si>
+  <si>
+    <t>remember; licking doorknobs is illegal on other planets</t>
+  </si>
+  <si>
+    <t>figure it out</t>
+  </si>
+  <si>
+    <t>kick the ball</t>
+  </si>
+  <si>
+    <t>ponder that for a moment</t>
+  </si>
+  <si>
+    <t>should we vote on it?</t>
   </si>
 </sst>
 </file>
@@ -900,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F77214D8-39E6-4145-A9FC-AB6165C9285C}">
-  <dimension ref="A1:N23"/>
+  <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -922,9 +949,10 @@
     <col min="12" max="12" width="33.6640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="43.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="47" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -967,8 +995,11 @@
       <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O1" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>121</v>
       </c>
@@ -1011,8 +1042,11 @@
       <c r="N2" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>114</v>
       </c>
@@ -1055,8 +1089,11 @@
       <c r="N3" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O3" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>110</v>
       </c>
@@ -1099,8 +1136,11 @@
       <c r="N4" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O4" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -1140,8 +1180,11 @@
       <c r="N5" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O5" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>41</v>
       </c>
@@ -1181,8 +1224,11 @@
       <c r="N6" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O6" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>58</v>
       </c>
@@ -1222,8 +1268,11 @@
       <c r="N7" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O7" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>124</v>
       </c>
@@ -1254,8 +1303,11 @@
       <c r="M8" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O8" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>49</v>
       </c>
@@ -1286,8 +1338,11 @@
       <c r="M9" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O9" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>67</v>
       </c>
@@ -1313,7 +1368,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>75</v>
       </c>
@@ -1336,7 +1391,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>83</v>
       </c>
@@ -1353,7 +1408,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>117</v>
       </c>
@@ -1370,7 +1425,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>100</v>
       </c>
@@ -1387,7 +1442,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>90</v>
       </c>
@@ -1401,7 +1456,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>

</xml_diff>